<commit_message>
inserting products into database & displaying on website
</commit_message>
<xml_diff>
--- a/admin_area/Menu.xlsx
+++ b/admin_area/Menu.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14080" tabRatio="500"/>
+    <workbookView xWindow="9160" yWindow="3960" windowWidth="16440" windowHeight="10580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
   <si>
     <t>Vnese</t>
   </si>
@@ -225,13 +226,106 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>1. Build a website</t>
+  </si>
+  <si>
+    <t>Your website is the heart of your restaurant’s brand. It should be eye-catching, yet easy to navigate. Make sure it contains these items:</t>
+  </si>
+  <si>
+    <t>An easy-to-ready menu — you can use an app such as OpenMenu to manage and share yours</t>
+  </si>
+  <si>
+    <t>Featured food items, including a description and nutrition information</t>
+  </si>
+  <si>
+    <t>Newsletter sign-up box</t>
+  </si>
+  <si>
+    <t>Order online button for pickup orders</t>
+  </si>
+  <si>
+    <t>Reservation button</t>
+  </si>
+  <si>
+    <t>Social media icons that link to your social pages</t>
+  </si>
+  <si>
+    <t>Rewards</t>
+  </si>
+  <si>
+    <t>Gift cards</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Disclaimer</t>
+  </si>
+  <si>
+    <t>Careers</t>
+  </si>
+  <si>
+    <t>Newsroom</t>
+  </si>
+  <si>
+    <r>
+      <t>Editor’s note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF1D1D1B"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t> Still in need of a site? Consider </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF00A63F"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>GoDaddy’s GoCentral Website Builder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF1D1D1B"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>. You can create an online presence in less than an hour, complete with a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF00A63F"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>beautiful menu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF1D1D1B"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t> and industry-specific layouts and imagery.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -243,6 +337,35 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18.7"/>
+      <color rgb="FF1D1D1B"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF1D1D1B"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF00A63F"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF1D1D1B"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -332,10 +455,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -359,8 +483,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -638,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1277,4 +1406,110 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A8" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>